<commit_message>
Fixed .gitignore to rename "wormpy" to "src"
Also made a slight revision to the Code Progress document
</commit_message>
<xml_diff>
--- a/documentation/Code Progress.xlsx
+++ b/documentation/Code Progress.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -167,15 +162,9 @@
     <t>Note: Only the movement_validation repo is being actively worked on.  This is intended to be the finished product for use by scientists and by OpenWorm.</t>
   </si>
   <si>
-    <t>Note: "yes" / "no" refers to whether that code compenent has been implemented.</t>
-  </si>
-  <si>
     <t>Pre-Features* (inc. Normalization)</t>
   </si>
   <si>
-    <t>not yet compared</t>
-  </si>
-  <si>
     <t>GUI</t>
   </si>
   <si>
@@ -189,6 +178,12 @@
   </si>
   <si>
     <t>* The original Yemini code stored simply-calculated features like width and skeleton along with the segmented contour, as a part of the machine vision step.  Here we show this as a separate step, since we will need to calculate these ourselves if we are supplied only contour data from Geppetto.  Also included here in the pre-features step is the reducing of the number of points lengthwise on the worm to just 49 (the "normalized" worm).</t>
+  </si>
+  <si>
+    <t>Note: "yes" / "no" refers to whether that code component has been implemented.</t>
+  </si>
+  <si>
+    <t>may be compared</t>
   </si>
 </sst>
 </file>
@@ -366,6 +361,33 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,33 +399,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,13 +571,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>501650</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>501650</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>561975</xdr:rowOff>
     </xdr:to>
@@ -593,7 +588,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10134600" y="2495550"/>
+          <a:off x="11245850" y="3117850"/>
           <a:ext cx="0" cy="542925"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -624,13 +619,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>488950</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>488950</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>561975</xdr:rowOff>
     </xdr:to>
@@ -641,7 +636,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10134600" y="1352550"/>
+          <a:off x="11233150" y="1974850"/>
           <a:ext cx="0" cy="542925"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1167,7 +1162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1180,7 +1175,9 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1196,18 +1193,18 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E3" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="27" t="s">
-        <v>51</v>
+      <c r="E3" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1233,7 +1230,7 @@
         <v>31</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>2</v>
@@ -1247,8 +1244,8 @@
       <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="28" t="s">
-        <v>50</v>
+      <c r="M4" s="23" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,8 +1305,8 @@
       <c r="K6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="25"/>
-      <c r="M6" s="29"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1348,7 +1345,7 @@
       <c r="L7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="30" t="s">
+      <c r="M7" s="25" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1374,19 +1371,19 @@
       <c r="K8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="26"/>
-      <c r="M8" s="31" t="s">
+      <c r="L8" s="21"/>
+      <c r="M8" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -1401,29 +1398,29 @@
       <c r="G9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="23" t="s">
+      <c r="I9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="M9" s="27" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="14" t="s">
         <v>30</v>
       </c>
@@ -1436,20 +1433,20 @@
       <c r="G10" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
     </row>
     <row r="11" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="9"/>
       <c r="G11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="18" t="s">
-        <v>49</v>
+      <c r="I11" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -1496,97 +1493,92 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
+      <c r="A14" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
+      <c r="A15" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
+      <c r="A16" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A15:M15"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="A17:M17"/>
     <mergeCell ref="A18:M18"/>
     <mergeCell ref="E3:L3"/>
     <mergeCell ref="A9:A10"/>
@@ -1597,6 +1589,11 @@
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="J9:J10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="A17:M17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Small edit to code progress document
</commit_message>
<xml_diff>
--- a/documentation/Code Progress.xlsx
+++ b/documentation/Code Progress.xlsx
@@ -66,9 +66,6 @@
     <t>(Michael working on this)</t>
   </si>
   <si>
-    <t>(Manuel working on this)</t>
-  </si>
-  <si>
     <t>Fitness Function</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>may be compared</t>
+  </si>
+  <si>
+    <t>(Miguel working on this)</t>
   </si>
 </sst>
 </file>
@@ -382,9 +382,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -398,6 +395,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1162,7 +1162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1175,9 +1175,7 @@
   </sheetPr>
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1189,36 +1187,36 @@
   <sheetData>
     <row r="1" spans="1:13" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A1" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E3" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="E3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
@@ -1227,25 +1225,25 @@
         <v>1</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M4" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1259,13 +1257,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>13</v>
@@ -1277,13 +1275,13 @@
         <v>13</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M5" s="13" t="s">
         <v>13</v>
@@ -1299,11 +1297,11 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="24"/>
@@ -1319,34 +1317,34 @@
         <v>9</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M7" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1356,226 +1354,226 @@
       <c r="D8" s="2"/>
       <c r="E8" s="8"/>
       <c r="F8" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J8" s="18"/>
       <c r="K8" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="31" t="s">
+      <c r="J9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="L9" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="27" t="s">
-        <v>28</v>
+      <c r="L9" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
     </row>
     <row r="11" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="9"/>
       <c r="G11" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
     </row>
     <row r="12" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
+      <c r="A14" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="A15" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
+      <c r="A16" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="A17" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
+      <c r="A18" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>